<commit_message>
corrected airport list files
</commit_message>
<xml_diff>
--- a/static/download/2022/RP3_APT_ASMA_2022_Jan_Feb.xlsx
+++ b/static/download/2022/RP3_APT_ASMA_2022_Jan_Feb.xlsx
@@ -1,26 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hhegendo\Downloads\04-release-20220413T145423Z-001\04-release\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12000"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <workbookPr/>
   <sheets>
-    <sheet name="ASMA_APT" sheetId="1" r:id="rId1"/>
-    <sheet name="Change Log" sheetId="2" r:id="rId2"/>
+    <sheet state="visible" name="ASMA_APT" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="Change Log" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="127">
   <si>
     <t>Data source</t>
   </si>
@@ -85,7 +77,7 @@
     <t>Belgium</t>
   </si>
   <si>
-    <t>Berlin/ Schoenefeld (EDDB)</t>
+    <t>Berlin Brandenburg (EDDB)</t>
   </si>
   <si>
     <t>EDDB</t>
@@ -406,79 +398,78 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="d&quot; &quot;mmm&quot; &quot;yyyy"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="166" formatCode="d\ mmm\ yyyy"/>
+    <numFmt numFmtId="166" formatCode="d mmm yyyy"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="9"/>
+      <sz val="9.0"/>
       <color rgb="FF396EA2"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="9.0"/>
       <color rgb="FF396EA2"/>
       <name val="Calibri"/>
     </font>
     <font>
       <u/>
-      <sz val="9"/>
+      <sz val="9.0"/>
       <color rgb="FF396EA2"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="9.0"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <u/>
-      <sz val="9"/>
+      <sz val="9.0"/>
       <color rgb="FF396EA2"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="9"/>
+      <sz val="9.0"/>
       <color rgb="FF980000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="9.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="8"/>
+      <sz val="8.0"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="8.0"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="10"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="9.0"/>
       <color rgb="FFF3F3F3"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="9.0"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -487,7 +478,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -509,43 +500,27 @@
     </fill>
   </fills>
   <borders count="8">
+    <border/>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -554,25 +529,18 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
+    </border>
+    <border>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -587,400 +555,174 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
   <cellXfs count="42">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="7" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="7" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="4" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="6" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="7" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="7" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="7" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="7" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="7" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="7" numFmtId="2" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="12" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="17" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="12" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472C4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="5.0" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B7" sqref="B7" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="5" width="22.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="20.5"/>
+    <col customWidth="1" min="2" max="2" width="15.5"/>
+    <col customWidth="1" min="3" max="3" width="13.25"/>
+    <col customWidth="1" min="4" max="5" width="22.75"/>
+    <col customWidth="1" min="6" max="6" width="18.13"/>
+    <col customWidth="1" min="7" max="7" width="20.75"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" ht="12.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -992,7 +734,7 @@
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="5">
-        <v>44562</v>
+        <v>44562.0</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>3</v>
@@ -1002,19 +744,19 @@
         <v>ASMA additional time</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="9">
-        <v>44664</v>
+        <v>44664.0</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="12">
-        <v>44620</v>
+        <v>44620.0</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>6</v>
@@ -1023,7 +765,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" ht="12.75" customHeight="1">
       <c r="A3" s="15" t="s">
         <v>8</v>
       </c>
@@ -1033,11 +775,8 @@
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
-      <c r="I3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" ht="12.75" customHeight="1">
       <c r="A4" s="17" t="s">
         <v>9</v>
       </c>
@@ -1050,7 +789,7 @@
       <c r="F4" s="21"/>
       <c r="G4" s="21"/>
     </row>
-    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" ht="12.75" customHeight="1">
       <c r="A5" s="22" t="s">
         <v>11</v>
       </c>
@@ -1073,7 +812,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="24" t="s">
         <v>18</v>
       </c>
@@ -1084,11 +823,11 @@
         <v>20</v>
       </c>
       <c r="D6" s="27">
-        <v>5005</v>
+        <v>5005.0</v>
       </c>
       <c r="E6" s="28">
-        <f t="shared" ref="E6:E9" si="0">F6/D6</f>
-        <v>0.75360239760239767</v>
+        <f t="shared" ref="E6:E9" si="1">F6/D6</f>
+        <v>0.7536023976</v>
       </c>
       <c r="F6" s="27">
         <v>3771.78</v>
@@ -1097,7 +836,7 @@
         <v>12.67</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" ht="12.75" customHeight="1">
       <c r="A7" s="24" t="s">
         <v>21</v>
       </c>
@@ -1108,11 +847,11 @@
         <v>23</v>
       </c>
       <c r="D7" s="27">
-        <v>9187</v>
+        <v>9187.0</v>
       </c>
       <c r="E7" s="28">
-        <f t="shared" si="0"/>
-        <v>1.1191379122673344</v>
+        <f t="shared" si="1"/>
+        <v>1.119137912</v>
       </c>
       <c r="F7" s="27">
         <v>10281.52</v>
@@ -1121,7 +860,7 @@
         <v>14.08</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="24" t="s">
         <v>24</v>
       </c>
@@ -1132,11 +871,11 @@
         <v>23</v>
       </c>
       <c r="D8" s="27">
-        <v>12063</v>
+        <v>12063.0</v>
       </c>
       <c r="E8" s="28">
-        <f t="shared" si="0"/>
-        <v>1.8069568100804112</v>
+        <f t="shared" si="1"/>
+        <v>1.80695681</v>
       </c>
       <c r="F8" s="27">
         <v>21797.32</v>
@@ -1145,7 +884,7 @@
         <v>13.83</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="24" t="s">
         <v>26</v>
       </c>
@@ -1156,11 +895,11 @@
         <v>23</v>
       </c>
       <c r="D9" s="27">
-        <v>5045</v>
+        <v>5045.0</v>
       </c>
       <c r="E9" s="28">
-        <f t="shared" si="0"/>
-        <v>0.6719801783944499</v>
+        <f t="shared" si="1"/>
+        <v>0.6719801784</v>
       </c>
       <c r="F9" s="27">
         <v>3390.14</v>
@@ -1169,7 +908,7 @@
         <v>13.97</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="24" t="s">
         <v>28</v>
       </c>
@@ -1184,7 +923,7 @@
       <c r="F10" s="27"/>
       <c r="G10" s="29"/>
     </row>
-    <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" ht="12.75" customHeight="1">
       <c r="A11" s="24" t="s">
         <v>30</v>
       </c>
@@ -1195,11 +934,11 @@
         <v>23</v>
       </c>
       <c r="D11" s="27">
-        <v>3454</v>
+        <v>3454.0</v>
       </c>
       <c r="E11" s="28">
-        <f t="shared" ref="E11:E17" si="1">F11/D11</f>
-        <v>0.71152866242038215</v>
+        <f t="shared" ref="E11:E17" si="2">F11/D11</f>
+        <v>0.7115286624</v>
       </c>
       <c r="F11" s="27">
         <v>2457.62</v>
@@ -1208,7 +947,7 @@
         <v>12.72</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" ht="12.75" customHeight="1">
       <c r="A12" s="24" t="s">
         <v>32</v>
       </c>
@@ -1219,11 +958,11 @@
         <v>23</v>
       </c>
       <c r="D12" s="27">
-        <v>15174</v>
+        <v>15174.0</v>
       </c>
       <c r="E12" s="28">
-        <f t="shared" si="1"/>
-        <v>1.389280347963622</v>
+        <f t="shared" si="2"/>
+        <v>1.389280348</v>
       </c>
       <c r="F12" s="27">
         <v>21080.94</v>
@@ -1232,7 +971,7 @@
         <v>13.17</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" ht="12.75" customHeight="1">
       <c r="A13" s="24" t="s">
         <v>34</v>
       </c>
@@ -1243,11 +982,11 @@
         <v>23</v>
       </c>
       <c r="D13" s="27">
-        <v>1602</v>
+        <v>1602.0</v>
       </c>
       <c r="E13" s="28">
-        <f t="shared" si="1"/>
-        <v>0.58468789013732836</v>
+        <f t="shared" si="2"/>
+        <v>0.5846878901</v>
       </c>
       <c r="F13" s="27">
         <v>936.67</v>
@@ -1256,7 +995,7 @@
         <v>12.75</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" ht="12.75" customHeight="1">
       <c r="A14" s="24" t="s">
         <v>36</v>
       </c>
@@ -1267,11 +1006,11 @@
         <v>38</v>
       </c>
       <c r="D14" s="27">
-        <v>8001</v>
+        <v>8001.0</v>
       </c>
       <c r="E14" s="28">
-        <f t="shared" si="1"/>
-        <v>1.294923134608174</v>
+        <f t="shared" si="2"/>
+        <v>1.294923135</v>
       </c>
       <c r="F14" s="27">
         <v>10360.68</v>
@@ -1280,7 +1019,7 @@
         <v>12.44</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" ht="12.75" customHeight="1">
       <c r="A15" s="24" t="s">
         <v>39</v>
       </c>
@@ -1291,20 +1030,20 @@
         <v>41</v>
       </c>
       <c r="D15" s="27">
-        <v>13203</v>
+        <v>13203.0</v>
       </c>
       <c r="E15" s="28">
-        <f t="shared" si="1"/>
-        <v>1.4431871544345982</v>
+        <f t="shared" si="2"/>
+        <v>1.443187154</v>
       </c>
       <c r="F15" s="27">
-        <v>19054.400000000001</v>
+        <v>19054.4</v>
       </c>
       <c r="G15" s="28">
         <v>13.42</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" ht="12.75" customHeight="1">
       <c r="A16" s="24" t="s">
         <v>42</v>
       </c>
@@ -1315,11 +1054,11 @@
         <v>44</v>
       </c>
       <c r="D16" s="27">
-        <v>5329</v>
+        <v>5329.0</v>
       </c>
       <c r="E16" s="28">
-        <f t="shared" si="1"/>
-        <v>0.97232689059861133</v>
+        <f t="shared" si="2"/>
+        <v>0.9723268906</v>
       </c>
       <c r="F16" s="27">
         <v>5181.53</v>
@@ -1328,7 +1067,7 @@
         <v>11.68</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" ht="12.75" customHeight="1">
       <c r="A17" s="24" t="s">
         <v>45</v>
       </c>
@@ -1339,11 +1078,11 @@
         <v>47</v>
       </c>
       <c r="D17" s="27">
-        <v>5406</v>
+        <v>5406.0</v>
       </c>
       <c r="E17" s="28">
-        <f t="shared" si="1"/>
-        <v>0.96424528301886792</v>
+        <f t="shared" si="2"/>
+        <v>0.964245283</v>
       </c>
       <c r="F17" s="27">
         <v>5212.71</v>
@@ -1352,7 +1091,7 @@
         <v>13.05</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" ht="12.75" customHeight="1">
       <c r="A18" s="24" t="s">
         <v>48</v>
       </c>
@@ -1367,7 +1106,7 @@
       <c r="F18" s="27"/>
       <c r="G18" s="29"/>
     </row>
-    <row r="19" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" ht="12.75" customHeight="1">
       <c r="A19" s="24" t="s">
         <v>51</v>
       </c>
@@ -1378,20 +1117,20 @@
         <v>50</v>
       </c>
       <c r="D19" s="27">
-        <v>10441</v>
+        <v>10441.0</v>
       </c>
       <c r="E19" s="28">
         <f>F19/D19</f>
-        <v>0.78966286754142334</v>
+        <v>0.7896628675</v>
       </c>
       <c r="F19" s="27">
-        <v>8244.8700000000008</v>
+        <v>8244.87</v>
       </c>
       <c r="G19" s="28">
         <v>12.87</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" ht="12.75" customHeight="1">
       <c r="A20" s="24" t="s">
         <v>53</v>
       </c>
@@ -1406,7 +1145,7 @@
       <c r="F20" s="27"/>
       <c r="G20" s="29"/>
     </row>
-    <row r="21" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" ht="12.75" customHeight="1">
       <c r="A21" s="24" t="s">
         <v>56</v>
       </c>
@@ -1417,11 +1156,11 @@
         <v>58</v>
       </c>
       <c r="D21" s="27">
-        <v>9014</v>
+        <v>9014.0</v>
       </c>
       <c r="E21" s="28">
-        <f t="shared" ref="E21:E25" si="2">F21/D21</f>
-        <v>0.93716995784335477</v>
+        <f t="shared" ref="E21:E25" si="3">F21/D21</f>
+        <v>0.9371699578</v>
       </c>
       <c r="F21" s="27">
         <v>8447.65</v>
@@ -1430,7 +1169,7 @@
         <v>13.19</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" ht="12.75" customHeight="1">
       <c r="A22" s="24" t="s">
         <v>59</v>
       </c>
@@ -1441,11 +1180,11 @@
         <v>61</v>
       </c>
       <c r="D22" s="27">
-        <v>7100</v>
+        <v>7100.0</v>
       </c>
       <c r="E22" s="28">
-        <f t="shared" si="2"/>
-        <v>1.2448042253521128</v>
+        <f t="shared" si="3"/>
+        <v>1.244804225</v>
       </c>
       <c r="F22" s="27">
         <v>8838.11</v>
@@ -1454,7 +1193,7 @@
         <v>14.75</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" ht="12.75" customHeight="1">
       <c r="A23" s="24" t="s">
         <v>62</v>
       </c>
@@ -1465,11 +1204,11 @@
         <v>61</v>
       </c>
       <c r="D23" s="27">
-        <v>4161</v>
+        <v>4161.0</v>
       </c>
       <c r="E23" s="28">
-        <f t="shared" si="2"/>
-        <v>0.58111992309540972</v>
+        <f t="shared" si="3"/>
+        <v>0.5811199231</v>
       </c>
       <c r="F23" s="27">
         <v>2418.04</v>
@@ -1478,7 +1217,7 @@
         <v>14.17</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" ht="12.75" customHeight="1">
       <c r="A24" s="24" t="s">
         <v>64</v>
       </c>
@@ -1489,11 +1228,11 @@
         <v>61</v>
       </c>
       <c r="D24" s="27">
-        <v>14730</v>
+        <v>14730.0</v>
       </c>
       <c r="E24" s="28">
-        <f t="shared" si="2"/>
-        <v>1.0382932790224033</v>
+        <f t="shared" si="3"/>
+        <v>1.038293279</v>
       </c>
       <c r="F24" s="27">
         <v>15294.06</v>
@@ -1502,7 +1241,7 @@
         <v>13.08</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" ht="12.75" customHeight="1">
       <c r="A25" s="24" t="s">
         <v>66</v>
       </c>
@@ -1513,11 +1252,11 @@
         <v>61</v>
       </c>
       <c r="D25" s="27">
-        <v>22348</v>
+        <v>22348.0</v>
       </c>
       <c r="E25" s="28">
-        <f t="shared" si="2"/>
-        <v>0.6673608376588509</v>
+        <f t="shared" si="3"/>
+        <v>0.6673608377</v>
       </c>
       <c r="F25" s="27">
         <v>14914.18</v>
@@ -1526,7 +1265,7 @@
         <v>12.93</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" ht="12.75" customHeight="1">
       <c r="A26" s="24" t="s">
         <v>68</v>
       </c>
@@ -1541,7 +1280,7 @@
       <c r="F26" s="27"/>
       <c r="G26" s="29"/>
     </row>
-    <row r="27" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" ht="12.75" customHeight="1">
       <c r="A27" s="24" t="s">
         <v>70</v>
       </c>
@@ -1552,11 +1291,11 @@
         <v>61</v>
       </c>
       <c r="D27" s="27">
-        <v>5434</v>
+        <v>5434.0</v>
       </c>
       <c r="E27" s="28">
-        <f t="shared" ref="E27:E29" si="3">F27/D27</f>
-        <v>0.39036253220463746</v>
+        <f t="shared" ref="E27:E29" si="4">F27/D27</f>
+        <v>0.3903625322</v>
       </c>
       <c r="F27" s="27">
         <v>2121.23</v>
@@ -1565,7 +1304,7 @@
         <v>13.21</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" ht="12.75" customHeight="1">
       <c r="A28" s="24" t="s">
         <v>72</v>
       </c>
@@ -1576,11 +1315,11 @@
         <v>74</v>
       </c>
       <c r="D28" s="27">
-        <v>3828</v>
+        <v>3828.0</v>
       </c>
       <c r="E28" s="28">
-        <f t="shared" si="3"/>
-        <v>0.42128526645768027</v>
+        <f t="shared" si="4"/>
+        <v>0.4212852665</v>
       </c>
       <c r="F28" s="27">
         <v>1612.68</v>
@@ -1589,7 +1328,7 @@
         <v>13.24</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" ht="12.75" customHeight="1">
       <c r="A29" s="24" t="s">
         <v>75</v>
       </c>
@@ -1600,11 +1339,11 @@
         <v>74</v>
       </c>
       <c r="D29" s="27">
-        <v>2072</v>
+        <v>2072.0</v>
       </c>
       <c r="E29" s="28">
-        <f t="shared" si="3"/>
-        <v>0.61519305019305026</v>
+        <f t="shared" si="4"/>
+        <v>0.6151930502</v>
       </c>
       <c r="F29" s="27">
         <v>1274.68</v>
@@ -1613,7 +1352,7 @@
         <v>12.85</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" ht="12.75" customHeight="1">
       <c r="A30" s="24" t="s">
         <v>77</v>
       </c>
@@ -1628,7 +1367,7 @@
       <c r="F30" s="27"/>
       <c r="G30" s="29"/>
     </row>
-    <row r="31" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" ht="12.75" customHeight="1">
       <c r="A31" s="24" t="s">
         <v>79</v>
       </c>
@@ -1639,11 +1378,11 @@
         <v>74</v>
       </c>
       <c r="D31" s="27">
-        <v>6509</v>
+        <v>6509.0</v>
       </c>
       <c r="E31" s="28">
-        <f t="shared" ref="E31:E33" si="4">F31/D31</f>
-        <v>1.0012275311107697</v>
+        <f t="shared" ref="E31:E33" si="5">F31/D31</f>
+        <v>1.001227531</v>
       </c>
       <c r="F31" s="27">
         <v>6516.99</v>
@@ -1652,7 +1391,7 @@
         <v>13.62</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" ht="12.75" customHeight="1">
       <c r="A32" s="24" t="s">
         <v>81</v>
       </c>
@@ -1663,11 +1402,11 @@
         <v>74</v>
       </c>
       <c r="D32" s="27">
-        <v>23857</v>
+        <v>23857.0</v>
       </c>
       <c r="E32" s="28">
-        <f t="shared" si="4"/>
-        <v>0.93546799681435211</v>
+        <f t="shared" si="5"/>
+        <v>0.9354679968</v>
       </c>
       <c r="F32" s="27">
         <v>22317.46</v>
@@ -1676,7 +1415,7 @@
         <v>14.37</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" ht="12.75" customHeight="1">
       <c r="A33" s="24" t="s">
         <v>83</v>
       </c>
@@ -1687,11 +1426,11 @@
         <v>74</v>
       </c>
       <c r="D33" s="27">
-        <v>5474</v>
+        <v>5474.0</v>
       </c>
       <c r="E33" s="28">
-        <f t="shared" si="4"/>
-        <v>1.116967482645232</v>
+        <f t="shared" si="5"/>
+        <v>1.116967483</v>
       </c>
       <c r="F33" s="27">
         <v>6114.28</v>
@@ -1700,7 +1439,7 @@
         <v>13.77</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" ht="12.75" customHeight="1">
       <c r="A34" s="24" t="s">
         <v>85</v>
       </c>
@@ -1715,7 +1454,7 @@
       <c r="F34" s="27"/>
       <c r="G34" s="29"/>
     </row>
-    <row r="35" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" ht="12.75" customHeight="1">
       <c r="A35" s="24" t="s">
         <v>88</v>
       </c>
@@ -1726,11 +1465,11 @@
         <v>90</v>
       </c>
       <c r="D35" s="27">
-        <v>5602</v>
+        <v>5602.0</v>
       </c>
       <c r="E35" s="28">
-        <f t="shared" ref="E35:E40" si="5">F35/D35</f>
-        <v>0.52277043912888255</v>
+        <f t="shared" ref="E35:E40" si="6">F35/D35</f>
+        <v>0.5227704391</v>
       </c>
       <c r="F35" s="27">
         <v>2928.56</v>
@@ -1739,7 +1478,7 @@
         <v>14.13</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" ht="12.75" customHeight="1">
       <c r="A36" s="24" t="s">
         <v>91</v>
       </c>
@@ -1750,11 +1489,11 @@
         <v>93</v>
       </c>
       <c r="D36" s="27">
-        <v>10892</v>
+        <v>10892.0</v>
       </c>
       <c r="E36" s="28">
-        <f t="shared" si="5"/>
-        <v>1.2297401762761659</v>
+        <f t="shared" si="6"/>
+        <v>1.229740176</v>
       </c>
       <c r="F36" s="27">
         <v>13394.33</v>
@@ -1763,7 +1502,7 @@
         <v>12.86</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" ht="12.75" customHeight="1">
       <c r="A37" s="24" t="s">
         <v>94</v>
       </c>
@@ -1774,20 +1513,20 @@
         <v>93</v>
       </c>
       <c r="D37" s="27">
-        <v>5229</v>
+        <v>5229.0</v>
       </c>
       <c r="E37" s="28">
-        <f t="shared" si="5"/>
-        <v>0.99068846815834777</v>
+        <f t="shared" si="6"/>
+        <v>0.9906884682</v>
       </c>
       <c r="F37" s="27">
-        <v>5180.3100000000004</v>
+        <v>5180.31</v>
       </c>
       <c r="G37" s="28">
         <v>13.5</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" ht="12.75" customHeight="1">
       <c r="A38" s="24" t="s">
         <v>96</v>
       </c>
@@ -1798,11 +1537,11 @@
         <v>93</v>
       </c>
       <c r="D38" s="27">
-        <v>5866</v>
+        <v>5866.0</v>
       </c>
       <c r="E38" s="28">
-        <f t="shared" si="5"/>
-        <v>1.2064370951244459</v>
+        <f t="shared" si="6"/>
+        <v>1.206437095</v>
       </c>
       <c r="F38" s="27">
         <v>7076.96</v>
@@ -1811,7 +1550,7 @@
         <v>11.44</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" ht="12.75" customHeight="1">
       <c r="A39" s="24" t="s">
         <v>98</v>
       </c>
@@ -1822,11 +1561,11 @@
         <v>93</v>
       </c>
       <c r="D39" s="27">
-        <v>3248</v>
+        <v>3248.0</v>
       </c>
       <c r="E39" s="28">
-        <f t="shared" si="5"/>
-        <v>0.84487992610837437</v>
+        <f t="shared" si="6"/>
+        <v>0.8448799261</v>
       </c>
       <c r="F39" s="27">
         <v>2744.17</v>
@@ -1835,7 +1574,7 @@
         <v>11.46</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" ht="12.75" customHeight="1">
       <c r="A40" s="24" t="s">
         <v>100</v>
       </c>
@@ -1846,20 +1585,20 @@
         <v>93</v>
       </c>
       <c r="D40" s="27">
-        <v>10548</v>
+        <v>10548.0</v>
       </c>
       <c r="E40" s="28">
-        <f t="shared" si="5"/>
-        <v>0.86717481987106548</v>
+        <f t="shared" si="6"/>
+        <v>0.8671748199</v>
       </c>
       <c r="F40" s="27">
-        <v>9146.9599999999991</v>
+        <v>9146.96</v>
       </c>
       <c r="G40" s="28">
         <v>12.16</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" ht="12.75" customHeight="1">
       <c r="A41" s="24" t="s">
         <v>102</v>
       </c>
@@ -1874,7 +1613,7 @@
       <c r="F41" s="27"/>
       <c r="G41" s="29"/>
     </row>
-    <row r="42" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" ht="12.75" customHeight="1">
       <c r="A42" s="24" t="s">
         <v>105</v>
       </c>
@@ -1885,11 +1624,11 @@
         <v>107</v>
       </c>
       <c r="D42" s="27">
-        <v>10101</v>
+        <v>10101.0</v>
       </c>
       <c r="E42" s="28">
         <f>F42/D42</f>
-        <v>0.96565290565290562</v>
+        <v>0.9656529057</v>
       </c>
       <c r="F42" s="27">
         <v>9754.06</v>
@@ -1898,7 +1637,7 @@
         <v>12.7</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" ht="12.75" customHeight="1">
       <c r="A43" s="24" t="s">
         <v>108</v>
       </c>
@@ -1913,7 +1652,7 @@
       <c r="F43" s="27"/>
       <c r="G43" s="29"/>
     </row>
-    <row r="44" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" ht="12.75" customHeight="1">
       <c r="A44" s="24" t="s">
         <v>111</v>
       </c>
@@ -1924,11 +1663,11 @@
         <v>110</v>
       </c>
       <c r="D44" s="27">
-        <v>11975</v>
+        <v>11975.0</v>
       </c>
       <c r="E44" s="28">
-        <f t="shared" ref="E44:E45" si="6">F44/D44</f>
-        <v>1.4448108559498956</v>
+        <f t="shared" ref="E44:E45" si="7">F44/D44</f>
+        <v>1.444810856</v>
       </c>
       <c r="F44" s="27">
         <v>17301.61</v>
@@ -1937,7 +1676,7 @@
         <v>14.03</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" ht="12.75" customHeight="1">
       <c r="A45" s="24" t="s">
         <v>113</v>
       </c>
@@ -1948,11 +1687,11 @@
         <v>115</v>
       </c>
       <c r="D45" s="27">
-        <v>5418</v>
+        <v>5418.0</v>
       </c>
       <c r="E45" s="28">
-        <f t="shared" si="6"/>
-        <v>0.63067183462532295</v>
+        <f t="shared" si="7"/>
+        <v>0.6306718346</v>
       </c>
       <c r="F45" s="27">
         <v>3416.98</v>
@@ -1961,7 +1700,7 @@
         <v>12.82</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" ht="12.75" customHeight="1">
       <c r="A46" s="24" t="s">
         <v>116</v>
       </c>
@@ -1976,7 +1715,7 @@
       <c r="F46" s="27"/>
       <c r="G46" s="29"/>
     </row>
-    <row r="47" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" ht="12.75" customHeight="1">
       <c r="A47" s="24" t="s">
         <v>119</v>
       </c>
@@ -1987,11 +1726,11 @@
         <v>118</v>
       </c>
       <c r="D47" s="27">
-        <v>10929</v>
+        <v>10929.0</v>
       </c>
       <c r="E47" s="28">
         <f>F47/D47</f>
-        <v>1.8976072833745083</v>
+        <v>1.897607283</v>
       </c>
       <c r="F47" s="27">
         <v>20738.95</v>
@@ -2001,28 +1740,27 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="15.13" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="68.7109375" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="13.0"/>
+    <col customWidth="1" min="2" max="2" width="15.88"/>
+    <col customWidth="1" min="3" max="3" width="7.0"/>
+    <col customWidth="1" min="4" max="4" width="68.75"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" ht="12.75" customHeight="1">
       <c r="A1" s="31" t="s">
         <v>121</v>
       </c>
@@ -2036,9 +1774,9 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="33">
-        <v>44351</v>
+        <v>44351.0</v>
       </c>
       <c r="B2" s="34" t="s">
         <v>125</v>
@@ -2048,25 +1786,25 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" ht="12.75" customHeight="1">
       <c r="A3" s="36"/>
       <c r="B3" s="37"/>
       <c r="C3" s="38"/>
       <c r="D3" s="37"/>
     </row>
-    <row r="4" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" ht="12.75" customHeight="1">
       <c r="A4" s="33"/>
       <c r="B4" s="39"/>
       <c r="C4" s="35"/>
       <c r="D4" s="40"/>
     </row>
-    <row r="5" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" ht="12.75" customHeight="1">
       <c r="A5" s="41"/>
       <c r="B5" s="39"/>
       <c r="C5" s="35"/>
       <c r="D5" s="40"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>